<commit_message>
Parametric tools, filtration file names
- Made exhaust adapter fully parametric and exported to `/CAD/Templates` folder.
- Ditto LED Guide Channel.
- Exhaust adapter now has a larger fan exhaust duct coverage area to help keep it in place.
- Mass renamed filtration parts with appropriate names and updated `Part Codes`.
</commit_message>
<xml_diff>
--- a/BOM/Part Codes.xlsx
+++ b/BOM/Part Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BF1556-196B-4171-9F78-71E270B78403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF504B6-1D5F-4908-9933-A5D7B1B16D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="3" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
   <sheets>
     <sheet name="000 - Printed Parts" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="780">
   <si>
     <t>Component</t>
   </si>
@@ -2221,6 +2221,165 @@
   </si>
   <si>
     <t>Panel Mount Extension, USB Type A</t>
+  </si>
+  <si>
+    <t>PN816</t>
+  </si>
+  <si>
+    <t>PN817</t>
+  </si>
+  <si>
+    <t>EnviroSupply</t>
+  </si>
+  <si>
+    <t>Activated Carbon, Virgin Coconut, 4-8mm</t>
+  </si>
+  <si>
+    <t>French Press Filter, 4" (8 Cup)</t>
+  </si>
+  <si>
+    <t>PN818</t>
+  </si>
+  <si>
+    <t>Silicone Tubing, 5/8" ID</t>
+  </si>
+  <si>
+    <t>Quality varies, but 3/4" OD often comes out as 20mm</t>
+  </si>
+  <si>
+    <t>PN082</t>
+  </si>
+  <si>
+    <t>PN060</t>
+  </si>
+  <si>
+    <t>PN819</t>
+  </si>
+  <si>
+    <t>HEPA Cartridge, 72x20mm</t>
+  </si>
+  <si>
+    <t>PN200</t>
+  </si>
+  <si>
+    <t>PN201</t>
+  </si>
+  <si>
+    <t>PN202</t>
+  </si>
+  <si>
+    <t>Filtration</t>
+  </si>
+  <si>
+    <t>Fan Exhaust Adapter</t>
+  </si>
+  <si>
+    <t>Fan Intake Gasket</t>
+  </si>
+  <si>
+    <t>Fans</t>
+  </si>
+  <si>
+    <t>200 - Filtration - Fans - Exhaust Adapter (TPU).stl</t>
+  </si>
+  <si>
+    <t>201 - Filtration - Fans - Intake Gasket (TPU).stl</t>
+  </si>
+  <si>
+    <t>Fan Intake Duct</t>
+  </si>
+  <si>
+    <t>202 - Filtration - Fans - Intake Duct.stl</t>
+  </si>
+  <si>
+    <t>PN203</t>
+  </si>
+  <si>
+    <t>HEPA</t>
+  </si>
+  <si>
+    <t>Filter Sleeve</t>
+  </si>
+  <si>
+    <t>203 - Filtration - HEPA - Filter Sleeve.stl</t>
+  </si>
+  <si>
+    <t>PN204</t>
+  </si>
+  <si>
+    <t>HEPA Intake Duct</t>
+  </si>
+  <si>
+    <t>PETG/ABS</t>
+  </si>
+  <si>
+    <t>TPU/PETG</t>
+  </si>
+  <si>
+    <t>204 - Filtration - HEPA - Intake Duct.stl</t>
+  </si>
+  <si>
+    <t>FIltration</t>
+  </si>
+  <si>
+    <t>HEPA Latch (TPU)</t>
+  </si>
+  <si>
+    <t>205 - Filtration - HEPA - Latch (TPU).stl</t>
+  </si>
+  <si>
+    <t>PN205</t>
+  </si>
+  <si>
+    <t>PN210</t>
+  </si>
+  <si>
+    <t>AC Filter</t>
+  </si>
+  <si>
+    <t>PN211</t>
+  </si>
+  <si>
+    <t>PN212</t>
+  </si>
+  <si>
+    <t>Tank Filter Ring</t>
+  </si>
+  <si>
+    <t>Tank Lid</t>
+  </si>
+  <si>
+    <t>Tank, 50mm</t>
+  </si>
+  <si>
+    <t>210 - Filtration - AC Filter - Tank Lid.stl</t>
+  </si>
+  <si>
+    <t>212 - Filtration - AC Filter - Tank, 50mm.stl</t>
+  </si>
+  <si>
+    <t>211 - Filtration - AC Filter - Tank Filter Ring.stl</t>
+  </si>
+  <si>
+    <t>PN206</t>
+  </si>
+  <si>
+    <t>Tank Gasket (TPU)</t>
+  </si>
+  <si>
+    <t>206 - Filtration - AC Filter - Tank Gasket (TPU).stl</t>
+  </si>
+  <si>
+    <t>Vacuum filters for Kenmore EF-2</t>
+  </si>
+  <si>
+    <t>PN207</t>
+  </si>
+  <si>
+    <t>Base Stand</t>
+  </si>
+  <si>
+    <t>207 - Filtration - Misc - Base Stand.stl</t>
   </si>
 </sst>
 </file>
@@ -2350,8 +2509,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I83" totalsRowShown="0">
-  <autoFilter ref="A1:I83" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I94" totalsRowShown="0">
+  <autoFilter ref="A1:I94" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I83">
     <sortCondition ref="A1:A83"/>
   </sortState>
@@ -2420,8 +2579,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{38E36A69-6DC9-48C9-A844-2C9B61CC67B5}" name="Table4" displayName="Table4" ref="A1:G13" totalsRowShown="0">
-  <autoFilter ref="A1:G13" xr:uid="{25A20098-4797-4CED-8859-6F0B389C74C7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{38E36A69-6DC9-48C9-A844-2C9B61CC67B5}" name="Table4" displayName="Table4" ref="A1:G16" totalsRowShown="0">
+  <autoFilter ref="A1:G16" xr:uid="{25A20098-4797-4CED-8859-6F0B389C74C7}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4A8FA1ED-C774-4AAD-B05A-174EEF2A2E73}" name="ID"/>
     <tableColumn id="7" xr3:uid="{3E39557D-9C3C-44AB-93C6-569543574005}" name="Type"/>
@@ -2764,10 +2923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3943,8 +4102,8 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>60</v>
+      <c r="A44" t="s">
+        <v>736</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -4326,8 +4485,8 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>82</v>
+      <c r="A58" t="s">
+        <v>735</v>
       </c>
       <c r="B58" t="s">
         <v>98</v>
@@ -5020,6 +5179,292 @@
       </c>
       <c r="I83" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>739</v>
+      </c>
+      <c r="B84" t="s">
+        <v>742</v>
+      </c>
+      <c r="C84" t="s">
+        <v>745</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>743</v>
+      </c>
+      <c r="F84" t="s">
+        <v>757</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>740</v>
+      </c>
+      <c r="B85" t="s">
+        <v>742</v>
+      </c>
+      <c r="C85" t="s">
+        <v>745</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>744</v>
+      </c>
+      <c r="F85" t="s">
+        <v>757</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+      <c r="I85" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>741</v>
+      </c>
+      <c r="B86" t="s">
+        <v>742</v>
+      </c>
+      <c r="C86" t="s">
+        <v>745</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>748</v>
+      </c>
+      <c r="F86" t="s">
+        <v>756</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="I86" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>750</v>
+      </c>
+      <c r="B87" t="s">
+        <v>742</v>
+      </c>
+      <c r="C87" t="s">
+        <v>751</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>752</v>
+      </c>
+      <c r="F87" t="s">
+        <v>756</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="I87" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>754</v>
+      </c>
+      <c r="B88" t="s">
+        <v>742</v>
+      </c>
+      <c r="C88" t="s">
+        <v>751</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1</v>
+      </c>
+      <c r="E88" t="s">
+        <v>755</v>
+      </c>
+      <c r="F88" t="s">
+        <v>756</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="I88" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>762</v>
+      </c>
+      <c r="B89" t="s">
+        <v>759</v>
+      </c>
+      <c r="C89" t="s">
+        <v>751</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1</v>
+      </c>
+      <c r="E89" t="s">
+        <v>760</v>
+      </c>
+      <c r="F89" t="s">
+        <v>757</v>
+      </c>
+      <c r="G89">
+        <v>2</v>
+      </c>
+      <c r="I89" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>773</v>
+      </c>
+      <c r="B90" t="s">
+        <v>742</v>
+      </c>
+      <c r="C90" t="s">
+        <v>764</v>
+      </c>
+      <c r="D90" t="s">
+        <v>1</v>
+      </c>
+      <c r="E90" t="s">
+        <v>774</v>
+      </c>
+      <c r="F90" t="s">
+        <v>757</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="I90" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>777</v>
+      </c>
+      <c r="B91" t="s">
+        <v>742</v>
+      </c>
+      <c r="C91" t="s">
+        <v>36</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" t="s">
+        <v>778</v>
+      </c>
+      <c r="F91" t="s">
+        <v>756</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="I91" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>763</v>
+      </c>
+      <c r="B92" t="s">
+        <v>742</v>
+      </c>
+      <c r="C92" t="s">
+        <v>764</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" t="s">
+        <v>768</v>
+      </c>
+      <c r="F92" t="s">
+        <v>756</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="I92" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>765</v>
+      </c>
+      <c r="B93" t="s">
+        <v>742</v>
+      </c>
+      <c r="C93" t="s">
+        <v>764</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1</v>
+      </c>
+      <c r="E93" t="s">
+        <v>767</v>
+      </c>
+      <c r="F93" t="s">
+        <v>756</v>
+      </c>
+      <c r="G93">
+        <v>2</v>
+      </c>
+      <c r="I93" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>766</v>
+      </c>
+      <c r="B94" t="s">
+        <v>759</v>
+      </c>
+      <c r="C94" t="s">
+        <v>764</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1</v>
+      </c>
+      <c r="E94" t="s">
+        <v>769</v>
+      </c>
+      <c r="F94" t="s">
+        <v>756</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="I94" t="s">
+        <v>771</v>
       </c>
     </row>
   </sheetData>
@@ -5035,7 +5480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165D9D9B-2E8A-4F3A-99A1-C30DA8072019}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -6123,7 +6568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34FE8B7A-08B6-4B45-9B87-6CA9E22A21CF}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -6870,15 +7315,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C344C7D-81F0-47D9-B06F-CFAE20D2FF21}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
@@ -7130,8 +7575,82 @@
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="4"/>
+      <c r="A13" t="s">
+        <v>727</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>731</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="E13" t="s">
+        <v>524</v>
+      </c>
       <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>728</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>730</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="E14" t="s">
+        <v>729</v>
+      </c>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>732</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>733</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="E15" t="s">
+        <v>524</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>737</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>738</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="E16" t="s">
+        <v>524</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" t="s">
+        <v>776</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7146,13 +7665,18 @@
     <hyperlink ref="D12" r:id="rId9" xr:uid="{F3B6BC83-9180-404D-851A-5678063A8099}"/>
     <hyperlink ref="D10" r:id="rId10" xr:uid="{FB4EB383-4CD5-4EB3-B2B9-AF397A8EDB56}"/>
     <hyperlink ref="D11" r:id="rId11" xr:uid="{FBE1C8F6-66F8-457A-A62C-64FCBF4D632F}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{6F77AF9A-3C1B-485D-A22C-75FAB4852648}"/>
+    <hyperlink ref="D13" r:id="rId13" xr:uid="{B30CA32C-9F81-40A1-A7BC-A82677CA34A3}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{223983E8-84DB-4664-90CE-4689CF839FEA}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{BAF7083F-A73F-46AC-A89B-9247B4580DD4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
   <ignoredErrors>
     <ignoredError sqref="F9" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>